<commit_message>
Combined process_accession with process_author titles; compared new and old combined_df
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/CCHF_Combined_10_29_saved.xlsx
+++ b/OutputData/CCHF/CCHF_Combined_10_29_saved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rshafer/Dropbox/GenBankRefs/OutputData/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD7F888-B33F-B142-A309-CC76DD6D72E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4EBF0-409C-E249-9081-935E78EA0F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="3240" windowWidth="40520" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20500" yWindow="4020" windowWidth="40520" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -10324,8 +10324,8 @@
   <dimension ref="A1:P368"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>